<commit_message>
remove addoc from pytest.ini
</commit_message>
<xml_diff>
--- a/tests/data_minimal_case/compounds_properties.xlsx
+++ b/tests/data_minimal_case/compounds_properties.xlsx
@@ -528,190 +528,190 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>naphthalene</t>
+          <t>phenol</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>naphthalene</t>
+          <t>phenol</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>C10H8</t>
+          <t>C6H6O</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>C1=CC=C2C=CC=CC2=C1</t>
+          <t>C1=CC=C(C=C1)O</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>128.17</v>
+        <v>94.11</v>
       </c>
       <c r="F2" t="n">
-        <v>3.3</v>
+        <v>1.5</v>
       </c>
       <c r="G2" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H2" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>0.9371147694468284</v>
+        <v>0.765763468281798</v>
       </c>
       <c r="K2" t="n">
-        <v>0.06291643910431459</v>
+        <v>0.06426522154925088</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>0.1700031877590054</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.000031208551143</v>
+        <v>0.8193178195728402</v>
       </c>
       <c r="R2" t="n">
-        <v>0</v>
+        <v>0.1807140580172139</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>phenol</t>
+          <t>dodecane</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>phenol</t>
+          <t>dodecane</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>C6H6O</t>
+          <t>C12H26</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>C1=CC=C(C=C1)O</t>
+          <t>CCCCCCCCCCCC</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>94.11</v>
+        <v>170.33</v>
       </c>
       <c r="F3" t="n">
-        <v>1.5</v>
+        <v>6.1</v>
       </c>
       <c r="G3" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H3" t="n">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.765763468281798</v>
+        <v>0.846192684788352</v>
       </c>
       <c r="K3" t="n">
-        <v>0.06426522154925088</v>
+        <v>0.1538660247754359</v>
       </c>
       <c r="L3" t="n">
-        <v>0.1700031877590054</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="N3" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>1.000058709563788</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.8193178195728402</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>0.1807140580172139</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>dodecane</t>
+          <t>naphthalene</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>dodecane</t>
+          <t>naphthalene</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>C12H26</t>
+          <t>C10H8</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCC</t>
+          <t>C1=CC=C2C=CC=CC2=C1</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>170.33</v>
+        <v>128.17</v>
       </c>
       <c r="F4" t="n">
-        <v>6.1</v>
+        <v>3.3</v>
       </c>
       <c r="G4" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H4" t="n">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.846192684788352</v>
+        <v>0.9371147694468284</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1538660247754359</v>
+        <v>0.06291643910431459</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O4" t="n">
         <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>1.000058709563788</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>1.000031208551143</v>
       </c>
       <c r="R4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
cleared __init__, added more in gcms.py, moved initialization in single tests added tests
</commit_message>
<xml_diff>
--- a/tests/data_minimal_case/compounds_properties.xlsx
+++ b/tests/data_minimal_case/compounds_properties.xlsx
@@ -528,126 +528,126 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>dodecane</t>
+          <t>phenol</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>dodecane</t>
+          <t>phenol</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>C12H26</t>
+          <t>C6H6O</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCC</t>
+          <t>C1=CC=C(C=C1)O</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>170.33</v>
+        <v>94.11</v>
       </c>
       <c r="F2" t="n">
-        <v>6.1</v>
+        <v>1.5</v>
       </c>
       <c r="G2" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H2" t="n">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>0.846192684788352</v>
+        <v>0.765763468281798</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1538660247754359</v>
+        <v>0.06426522154925088</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>0.1700031877590054</v>
       </c>
       <c r="M2" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2" t="n">
-        <v>1.000058709563788</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>0.8193178195728402</v>
       </c>
       <c r="R2" t="n">
-        <v>0</v>
+        <v>0.1807140580172139</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>naphthalene</t>
+          <t>dodecane</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>naphthalene</t>
+          <t>dodecane</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>C10H8</t>
+          <t>C12H26</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>C1=CC=C2C=CC=CC2=C1</t>
+          <t>CCCCCCCCCCCC</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>128.17</v>
+        <v>170.33</v>
       </c>
       <c r="F3" t="n">
-        <v>3.3</v>
+        <v>6.1</v>
       </c>
       <c r="G3" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H3" t="n">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.9371147694468284</v>
+        <v>0.846192684788352</v>
       </c>
       <c r="K3" t="n">
-        <v>0.06291643910431459</v>
+        <v>0.1538660247754359</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="N3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>1.000058709563788</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.000031208551143</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
         <v>0</v>
@@ -656,65 +656,65 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>phenol</t>
+          <t>naphthalene</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>phenol</t>
+          <t>naphthalene</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>C6H6O</t>
+          <t>C10H8</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>C1=CC=C(C=C1)O</t>
+          <t>C1=CC=C2C=CC=CC2=C1</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>94.11</v>
+        <v>128.17</v>
       </c>
       <c r="F4" t="n">
-        <v>1.5</v>
+        <v>3.3</v>
       </c>
       <c r="G4" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H4" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.765763468281798</v>
+        <v>0.9371147694468284</v>
       </c>
       <c r="K4" t="n">
-        <v>0.06426522154925088</v>
+        <v>0.06291643910431459</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1700031877590054</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="O4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.8193178195728402</v>
+        <v>1.000031208551143</v>
       </c>
       <c r="R4" t="n">
-        <v>0.1807140580172139</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added calibarion and semicalibration
</commit_message>
<xml_diff>
--- a/tests/data_minimal_case/compounds_properties.xlsx
+++ b/tests/data_minimal_case/compounds_properties.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,65 +471,85 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>el_Cl</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>el_H</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>el_O</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>el_mf_C</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>el_mf_Cl</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>el_mf_H</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>el_mf_O</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>fg_C-aliph</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>fg_C-arom</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>fg_Cl</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>fg_alcohol</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>fg_carboxyl</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>fg_mf_C-aliph</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>fg_mf_C-arom</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>fg_mf_Cl</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>fg_mf_alcohol</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>fg_mf_carboxyl</t>
         </is>
@@ -538,70 +558,82 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>naphthalene</t>
+          <t>dichlorobenzene</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>naphthalene</t>
+          <t>1,4-dichlorobenzene</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>C10H8</t>
+          <t>C6H4Cl2</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>C1=CC=C2C=CC=CC2=C1</t>
+          <t>C1=CC(=CC=C1Cl)Cl</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>128.17</v>
+        <v>147</v>
       </c>
       <c r="F2" t="n">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="G2" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H2" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J2" t="n">
-        <v>0.9371147694468284</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.06291643910431459</v>
+        <v>0.4902448979591837</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>0.4823129251700681</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>0.02742857142857143</v>
       </c>
       <c r="N2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R2" t="n">
-        <v>1.000031208551143</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
       </c>
       <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.517673469387755</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.4823129251700681</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -636,42 +668,54 @@
         <v>18</v>
       </c>
       <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
         <v>34</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>2</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.7653026548672566</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
         <v>0.121316814159292</v>
       </c>
-      <c r="L3" t="n">
+      <c r="N3" t="n">
         <v>0.1132672566371681</v>
       </c>
-      <c r="M3" t="n">
+      <c r="O3" t="n">
         <v>17</v>
       </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
       <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
         <v>1</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="T3" t="n">
         <v>0.8405345132743363</v>
       </c>
-      <c r="R3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="n">
         <v>0.1593522123893805</v>
       </c>
     </row>
@@ -704,60 +748,64 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>phenol</t>
+          <t>dodecane</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>phenol</t>
+          <t>dodecane</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>C6H6O</t>
+          <t>C12H26</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>C1=CC=C(C=C1)O</t>
+          <t>CCCCCCCCCCCC</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>94.11</v>
+        <v>170.33</v>
       </c>
       <c r="F5" t="n">
-        <v>1.5</v>
+        <v>6.1</v>
       </c>
       <c r="G5" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="J5" t="n">
-        <v>0.765763468281798</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.06426522154925088</v>
+        <v>0.846192684788352</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1700031877590054</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>0.1538660247754359</v>
       </c>
       <c r="N5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="P5" t="n">
         <v>0</v>
@@ -766,62 +814,74 @@
         <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>0.8193178195728402</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>0.1807140580172139</v>
+        <v>0</v>
       </c>
       <c r="T5" t="n">
+        <v>1.000058709563788</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>capric acid</t>
+          <t>naphthalene</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>decanoic acid</t>
+          <t>naphthalene</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>C10H20O2</t>
+          <t>C10H8</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>CCCCCCCCCC(=O)O</t>
+          <t>C1=CC=C2C=CC=CC2=C1</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>172.26</v>
+        <v>128.17</v>
       </c>
       <c r="F6" t="n">
-        <v>4.1</v>
+        <v>3.3</v>
       </c>
       <c r="G6" t="n">
         <v>10</v>
       </c>
       <c r="H6" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J6" t="n">
-        <v>0.6972599558806455</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.1170323928944619</v>
+        <v>0.9371147694468284</v>
       </c>
       <c r="L6" t="n">
-        <v>0.1857540926506444</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>9</v>
+        <v>0.06291643910431459</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
@@ -830,10 +890,10 @@
         <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.7387147335423198</v>
+        <v>0</v>
       </c>
       <c r="R6" t="n">
         <v>0</v>
@@ -842,77 +902,265 @@
         <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>0.2613317078834321</v>
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>1.000031208551143</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>dodecane</t>
+          <t>capric acid</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>dodecane</t>
+          <t>decanoic acid</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>C12H26</t>
+          <t>C10H20O2</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCC</t>
+          <t>CCCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>170.33</v>
+        <v>172.26</v>
       </c>
       <c r="F7" t="n">
-        <v>6.1</v>
+        <v>4.1</v>
       </c>
       <c r="G7" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H7" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J7" t="n">
-        <v>0.846192684788352</v>
+        <v>2</v>
       </c>
       <c r="K7" t="n">
-        <v>0.1538660247754359</v>
+        <v>0.6972599558806455</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>12</v>
+        <v>0.1170323928944619</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>0.1857540926506444</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="P7" t="n">
         <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>1.000058709563788</v>
+        <v>0</v>
       </c>
       <c r="R7" t="n">
         <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7" t="n">
-        <v>0</v>
+        <v>0.7387147335423198</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0.2613317078834321</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>phenol</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>phenol</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>C6H6O</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>C1=CC=C(C=C1)O</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>94.11</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G8" t="n">
+        <v>6</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>6</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.765763468281798</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.06426522154925088</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.1700031877590054</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>1</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.8193178195728402</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0.1807140580172139</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>palmitic acid</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>hexadecanoic acid</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>C16H32O2</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>CCCCCCCCCCCCCCCC(=O)O</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>256.42</v>
+      </c>
+      <c r="F9" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="G9" t="n">
+        <v>16</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>32</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.7494579205990172</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.125793619842446</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.1247874580765931</v>
+      </c>
+      <c r="O9" t="n">
+        <v>15</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>1</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.8244793697839481</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0.1755596287341081</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added samples creation and reports
</commit_message>
<xml_diff>
--- a/tests/data_minimal_case/compounds_properties.xlsx
+++ b/tests/data_minimal_case/compounds_properties.xlsx
@@ -558,254 +558,254 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>dichlorobenzene</t>
+          <t>notvalidcomp</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1,4-dichlorobenzene</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>C6H4Cl2</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>C1=CC(=CC=C1Cl)Cl</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>147</v>
-      </c>
-      <c r="F2" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="G2" t="n">
-        <v>6</v>
-      </c>
-      <c r="H2" t="n">
-        <v>2</v>
-      </c>
-      <c r="I2" t="n">
-        <v>4</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.4902448979591837</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.4823129251700681</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.02742857142857143</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>2</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0.517673469387755</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0.4823129251700681</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0</v>
-      </c>
+          <t>unidentified</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>oleic acid</t>
+          <t>dichlorobenzene</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>(z)-octadec-9-enoic acid</t>
+          <t>1,4-dichlorobenzene</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>C18H34O2</t>
+          <t>C6H4Cl2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
+          <t>C1=CC(=CC=C1Cl)Cl</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>282.5</v>
+        <v>147</v>
       </c>
       <c r="F3" t="n">
-        <v>6.5</v>
+        <v>3.4</v>
       </c>
       <c r="G3" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I3" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.4902448979591837</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.4823129251700681</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.02742857142857143</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q3" t="n">
         <v>2</v>
       </c>
-      <c r="K3" t="n">
-        <v>0.7653026548672566</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.121316814159292</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.1132672566371681</v>
-      </c>
-      <c r="O3" t="n">
-        <v>17</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
       <c r="R3" t="n">
         <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>0.8405345132743363</v>
+        <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>0</v>
+        <v>0.517673469387755</v>
       </c>
       <c r="V3" t="n">
-        <v>0</v>
+        <v>0.4823129251700681</v>
       </c>
       <c r="W3" t="n">
         <v>0</v>
       </c>
       <c r="X3" t="n">
-        <v>0.1593522123893805</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>notvalidcomp</t>
+          <t>phenol</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>unidentified</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
+          <t>phenol</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>C6H6O</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>C1=CC=C(C=C1)O</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>94.11</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G4" t="n">
+        <v>6</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>6</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.765763468281798</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.06426522154925088</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.1700031877590054</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.8193178195728402</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.1807140580172139</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>dodecane</t>
+          <t>palmitic acid</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>dodecane</t>
+          <t>hexadecanoic acid</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>C12H26</t>
+          <t>C16H32O2</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCC</t>
+          <t>CCCCCCCCCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>170.33</v>
+        <v>256.42</v>
       </c>
       <c r="F5" t="n">
-        <v>6.1</v>
+        <v>6.4</v>
       </c>
       <c r="G5" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K5" t="n">
-        <v>0.846192684788352</v>
+        <v>0.7494579205990172</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.1538660247754359</v>
+        <v>0.125793619842446</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>0.1247874580765931</v>
       </c>
       <c r="O5" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="P5" t="n">
         <v>0</v>
@@ -817,10 +817,10 @@
         <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5" t="n">
-        <v>1.000058709563788</v>
+        <v>0.8244793697839481</v>
       </c>
       <c r="U5" t="n">
         <v>0</v>
@@ -832,65 +832,65 @@
         <v>0</v>
       </c>
       <c r="X5" t="n">
-        <v>0</v>
+        <v>0.1755596287341081</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>naphthalene</t>
+          <t>dodecane</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>naphthalene</t>
+          <t>dodecane</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>C10H8</t>
+          <t>C12H26</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>C1=CC=C2C=CC=CC2=C1</t>
+          <t>CCCCCCCCCCCC</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>128.17</v>
+        <v>170.33</v>
       </c>
       <c r="F6" t="n">
-        <v>3.3</v>
+        <v>6.1</v>
       </c>
       <c r="G6" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9371147694468284</v>
+        <v>0.846192684788352</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>0.06291643910431459</v>
+        <v>0.1538660247754359</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="P6" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="n">
         <v>0</v>
@@ -902,10 +902,10 @@
         <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>0</v>
+        <v>1.000058709563788</v>
       </c>
       <c r="U6" t="n">
-        <v>1.000031208551143</v>
+        <v>0</v>
       </c>
       <c r="V6" t="n">
         <v>0</v>
@@ -1002,141 +1002,141 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>phenol</t>
+          <t>oleic acid</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>phenol</t>
+          <t>(z)-octadec-9-enoic acid</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>C6H6O</t>
+          <t>C18H34O2</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>C1=CC=C(C=C1)O</t>
+          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>94.11</v>
+        <v>282.5</v>
       </c>
       <c r="F8" t="n">
-        <v>1.5</v>
+        <v>6.5</v>
       </c>
       <c r="G8" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="J8" t="n">
+        <v>2</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.7653026548672566</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.121316814159292</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.1132672566371681</v>
+      </c>
+      <c r="O8" t="n">
+        <v>17</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
         <v>1</v>
       </c>
-      <c r="K8" t="n">
-        <v>0.765763468281798</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.06426522154925088</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.1700031877590054</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" t="n">
-        <v>1</v>
-      </c>
-      <c r="S8" t="n">
-        <v>0</v>
-      </c>
       <c r="T8" t="n">
-        <v>0</v>
+        <v>0.8405345132743363</v>
       </c>
       <c r="U8" t="n">
-        <v>0.8193178195728402</v>
+        <v>0</v>
       </c>
       <c r="V8" t="n">
         <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>0.1807140580172139</v>
+        <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>0</v>
+        <v>0.1593522123893805</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>palmitic acid</t>
+          <t>naphthalene</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>hexadecanoic acid</t>
+          <t>naphthalene</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>C16H32O2</t>
+          <t>C10H8</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCCCCCC(=O)O</t>
+          <t>C1=CC=C2C=CC=CC2=C1</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>256.42</v>
+        <v>128.17</v>
       </c>
       <c r="F9" t="n">
-        <v>6.4</v>
+        <v>3.3</v>
       </c>
       <c r="G9" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="J9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>0.7494579205990172</v>
+        <v>0.9371147694468284</v>
       </c>
       <c r="L9" t="n">
         <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>0.125793619842446</v>
+        <v>0.06291643910431459</v>
       </c>
       <c r="N9" t="n">
-        <v>0.1247874580765931</v>
+        <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q9" t="n">
         <v>0</v>
@@ -1145,13 +1145,13 @@
         <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T9" t="n">
-        <v>0.8244793697839481</v>
+        <v>0</v>
       </c>
       <c r="U9" t="n">
-        <v>0</v>
+        <v>1.000031208551143</v>
       </c>
       <c r="V9" t="n">
         <v>0</v>
@@ -1160,7 +1160,7 @@
         <v>0</v>
       </c>
       <c r="X9" t="n">
-        <v>0.1755596287341081</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added reports creation, saving
</commit_message>
<xml_diff>
--- a/tests/data_minimal_case/compounds_properties.xlsx
+++ b/tests/data_minimal_case/compounds_properties.xlsx
@@ -558,96 +558,144 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>notvalidcomp</t>
+          <t>capric acid</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>unidentified</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr"/>
+          <t>decanoic acid</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>C10H20O2</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CCCCCCCCCC(=O)O</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>172.26</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>20</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.6972599558806455</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.1170323928944619</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.1857540926506444</v>
+      </c>
+      <c r="O2" t="n">
+        <v>9</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.7387147335423198</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.2613317078834321</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>dichlorobenzene</t>
+          <t>dodecane</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1,4-dichlorobenzene</t>
+          <t>dodecane</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>C6H4Cl2</t>
+          <t>C12H26</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>C1=CC(=CC=C1Cl)Cl</t>
+          <t>CCCCCCCCCCCC</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>147</v>
+        <v>170.33</v>
       </c>
       <c r="F3" t="n">
-        <v>3.4</v>
+        <v>6.1</v>
       </c>
       <c r="G3" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.4902448979591837</v>
+        <v>0.846192684788352</v>
       </c>
       <c r="L3" t="n">
-        <v>0.4823129251700681</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0.02742857142857143</v>
+        <v>0.1538660247754359</v>
       </c>
       <c r="N3" t="n">
         <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="P3" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
         <v>0</v>
@@ -656,13 +704,13 @@
         <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>0</v>
+        <v>1.000058709563788</v>
       </c>
       <c r="U3" t="n">
-        <v>0.517673469387755</v>
+        <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>0.4823129251700681</v>
+        <v>0</v>
       </c>
       <c r="W3" t="n">
         <v>0</v>
@@ -674,84 +722,36 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>phenol</t>
+          <t>notvalidcomp</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>phenol</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>C6H6O</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>C1=CC=C(C=C1)O</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>94.11</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G4" t="n">
-        <v>6</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>6</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.765763468281798</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.06426522154925088</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.1700031877590054</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" t="n">
-        <v>1</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0</v>
-      </c>
-      <c r="T4" t="n">
-        <v>0</v>
-      </c>
-      <c r="U4" t="n">
-        <v>0.8193178195728402</v>
-      </c>
-      <c r="V4" t="n">
-        <v>0</v>
-      </c>
-      <c r="W4" t="n">
-        <v>0.1807140580172139</v>
-      </c>
-      <c r="X4" t="n">
-        <v>0</v>
-      </c>
+          <t>unidentified</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -838,56 +838,56 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>dodecane</t>
+          <t>oleic acid</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>dodecane</t>
+          <t>(z)-octadec-9-enoic acid</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>C12H26</t>
+          <t>C18H34O2</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCC</t>
+          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>170.33</v>
+        <v>282.5</v>
       </c>
       <c r="F6" t="n">
-        <v>6.1</v>
+        <v>6.5</v>
       </c>
       <c r="G6" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K6" t="n">
-        <v>0.846192684788352</v>
+        <v>0.7653026548672566</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>0.1538660247754359</v>
+        <v>0.121316814159292</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>0.1132672566371681</v>
       </c>
       <c r="O6" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="P6" t="n">
         <v>0</v>
@@ -899,10 +899,10 @@
         <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T6" t="n">
-        <v>1.000058709563788</v>
+        <v>0.8405345132743363</v>
       </c>
       <c r="U6" t="n">
         <v>0</v>
@@ -914,35 +914,35 @@
         <v>0</v>
       </c>
       <c r="X6" t="n">
-        <v>0</v>
+        <v>0.1593522123893805</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>capric acid</t>
+          <t>naphthalene</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>decanoic acid</t>
+          <t>naphthalene</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>C10H20O2</t>
+          <t>C10H8</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CCCCCCCCCC(=O)O</t>
+          <t>C1=CC=C2C=CC=CC2=C1</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>172.26</v>
+        <v>128.17</v>
       </c>
       <c r="F7" t="n">
-        <v>4.1</v>
+        <v>3.3</v>
       </c>
       <c r="G7" t="n">
         <v>10</v>
@@ -951,28 +951,28 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>0.6972599558806455</v>
+        <v>0.9371147694468284</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1170323928944619</v>
+        <v>0.06291643910431459</v>
       </c>
       <c r="N7" t="n">
-        <v>0.1857540926506444</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q7" t="n">
         <v>0</v>
@@ -981,13 +981,13 @@
         <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T7" t="n">
-        <v>0.7387147335423198</v>
+        <v>0</v>
       </c>
       <c r="U7" t="n">
-        <v>0</v>
+        <v>1.000031208551143</v>
       </c>
       <c r="V7" t="n">
         <v>0</v>
@@ -996,153 +996,153 @@
         <v>0</v>
       </c>
       <c r="X7" t="n">
-        <v>0.2613317078834321</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>oleic acid</t>
+          <t>dichlorobenzene</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>(z)-octadec-9-enoic acid</t>
+          <t>1,4-dichlorobenzene</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>C18H34O2</t>
+          <t>C6H4Cl2</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
+          <t>C1=CC(=CC=C1Cl)Cl</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>282.5</v>
+        <v>147</v>
       </c>
       <c r="F8" t="n">
-        <v>6.5</v>
+        <v>3.4</v>
       </c>
       <c r="G8" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I8" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.4902448979591837</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.4823129251700681</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.02742857142857143</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q8" t="n">
         <v>2</v>
       </c>
-      <c r="K8" t="n">
-        <v>0.7653026548672566</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.121316814159292</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.1132672566371681</v>
-      </c>
-      <c r="O8" t="n">
-        <v>17</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0</v>
-      </c>
       <c r="R8" t="n">
         <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>0.8405345132743363</v>
+        <v>0</v>
       </c>
       <c r="U8" t="n">
-        <v>0</v>
+        <v>0.517673469387755</v>
       </c>
       <c r="V8" t="n">
-        <v>0</v>
+        <v>0.4823129251700681</v>
       </c>
       <c r="W8" t="n">
         <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>0.1593522123893805</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>naphthalene</t>
+          <t>phenol</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>naphthalene</t>
+          <t>phenol</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>C10H8</t>
+          <t>C6H6O</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>C1=CC=C2C=CC=CC2=C1</t>
+          <t>C1=CC=C(C=C1)O</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>128.17</v>
+        <v>94.11</v>
       </c>
       <c r="F9" t="n">
-        <v>3.3</v>
+        <v>1.5</v>
       </c>
       <c r="G9" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>0.9371147694468284</v>
+        <v>0.765763468281798</v>
       </c>
       <c r="L9" t="n">
         <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>0.06291643910431459</v>
+        <v>0.06426522154925088</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>0.1700031877590054</v>
       </c>
       <c r="O9" t="n">
         <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="Q9" t="n">
         <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9" t="n">
         <v>0</v>
@@ -1151,13 +1151,13 @@
         <v>0</v>
       </c>
       <c r="U9" t="n">
-        <v>1.000031208551143</v>
+        <v>0.8193178195728402</v>
       </c>
       <c r="V9" t="n">
         <v>0</v>
       </c>
       <c r="W9" t="n">
-        <v>0</v>
+        <v>0.1807140580172139</v>
       </c>
       <c r="X9" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
added automatic method calling for all methods that depend on previous methods in the Project
</commit_message>
<xml_diff>
--- a/tests/data_minimal_case/compounds_properties.xlsx
+++ b/tests/data_minimal_case/compounds_properties.xlsx
@@ -558,59 +558,59 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>dodecane</t>
+          <t>naphthalene</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>dodecane</t>
+          <t>naphthalene</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>C12H26</t>
+          <t>C10H8</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCC</t>
+          <t>C1=CC=C2C=CC=CC2=C1</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>170.33</v>
+        <v>128.17</v>
       </c>
       <c r="F2" t="n">
-        <v>6.1</v>
+        <v>3.3</v>
       </c>
       <c r="G2" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.846192684788352</v>
+        <v>0.9371147694468284</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1538660247754359</v>
+        <v>0.06291643910431459</v>
       </c>
       <c r="N2" t="n">
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
@@ -622,10 +622,10 @@
         <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>1.000058709563788</v>
+        <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>0</v>
+        <v>1.000031208551143</v>
       </c>
       <c r="V2" t="n">
         <v>0</v>
@@ -640,56 +640,56 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>palmitic acid</t>
+          <t>dodecane</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>hexadecanoic acid</t>
+          <t>dodecane</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>C16H32O2</t>
+          <t>C12H26</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCCCCCC(=O)O</t>
+          <t>CCCCCCCCCCCC</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>256.42</v>
+        <v>170.33</v>
       </c>
       <c r="F3" t="n">
-        <v>6.4</v>
+        <v>6.1</v>
       </c>
       <c r="G3" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="J3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.7494579205990172</v>
+        <v>0.846192684788352</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0.125793619842446</v>
+        <v>0.1538660247754359</v>
       </c>
       <c r="N3" t="n">
-        <v>0.1247874580765931</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="P3" t="n">
         <v>0</v>
@@ -701,10 +701,10 @@
         <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>0.8244793697839481</v>
+        <v>1.000058709563788</v>
       </c>
       <c r="U3" t="n">
         <v>0</v>
@@ -716,7 +716,7 @@
         <v>0</v>
       </c>
       <c r="X3" t="n">
-        <v>0.1755596287341081</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -804,59 +804,59 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>naphthalene</t>
+          <t>oleic acid</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>naphthalene</t>
+          <t>(z)-octadec-9-enoic acid</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>C10H8</t>
+          <t>C18H34O2</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>C1=CC=C2C=CC=CC2=C1</t>
+          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>128.17</v>
+        <v>282.5</v>
       </c>
       <c r="F5" t="n">
-        <v>3.3</v>
+        <v>6.5</v>
       </c>
       <c r="G5" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K5" t="n">
-        <v>0.9371147694468284</v>
+        <v>0.7653026548672566</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.06291643910431459</v>
+        <v>0.121316814159292</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>0.1132672566371681</v>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="P5" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="n">
         <v>0</v>
@@ -865,13 +865,13 @@
         <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5" t="n">
-        <v>0</v>
+        <v>0.8405345132743363</v>
       </c>
       <c r="U5" t="n">
-        <v>1.000031208551143</v>
+        <v>0</v>
       </c>
       <c r="V5" t="n">
         <v>0</v>
@@ -880,206 +880,206 @@
         <v>0</v>
       </c>
       <c r="X5" t="n">
-        <v>0</v>
+        <v>0.1593522123893805</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>dichlorobenzene</t>
+          <t>palmitic acid</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1,4-dichlorobenzene</t>
+          <t>hexadecanoic acid</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>C6H4Cl2</t>
+          <t>C16H32O2</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>C1=CC(=CC=C1Cl)Cl</t>
+          <t>CCCCCCCCCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>147</v>
+        <v>256.42</v>
       </c>
       <c r="F6" t="n">
-        <v>3.4</v>
+        <v>6.4</v>
       </c>
       <c r="G6" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>32</v>
+      </c>
+      <c r="J6" t="n">
         <v>2</v>
       </c>
-      <c r="I6" t="n">
-        <v>4</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
       <c r="K6" t="n">
-        <v>0.4902448979591837</v>
+        <v>0.7494579205990172</v>
       </c>
       <c r="L6" t="n">
-        <v>0.4823129251700681</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>0.02742857142857143</v>
+        <v>0.125793619842446</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>0.1247874580765931</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P6" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R6" t="n">
         <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T6" t="n">
-        <v>0</v>
+        <v>0.8244793697839481</v>
       </c>
       <c r="U6" t="n">
-        <v>0.517673469387755</v>
+        <v>0</v>
       </c>
       <c r="V6" t="n">
-        <v>0.4823129251700681</v>
+        <v>0</v>
       </c>
       <c r="W6" t="n">
         <v>0</v>
       </c>
       <c r="X6" t="n">
-        <v>0</v>
+        <v>0.1755596287341081</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>notvalidcomp</t>
+          <t>p-dichlorobenzene</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>unidentified</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr"/>
-      <c r="X7" t="inlineStr"/>
+          <t>1,4-dichlorobenzene</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>C6H4Cl2</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>C1=CC(=CC=C1Cl)Cl</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>147</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="G7" t="n">
+        <v>6</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" t="n">
+        <v>4</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.4902448979591837</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.4823129251700681</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.02742857142857143</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>2</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.517673469387755</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.4823129251700681</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>oleic acid</t>
+          <t>notvalidcomp</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>(z)-octadec-9-enoic acid</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>C18H34O2</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>282.5</v>
-      </c>
-      <c r="F8" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="G8" t="n">
-        <v>18</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>34</v>
-      </c>
-      <c r="J8" t="n">
-        <v>2</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.7653026548672566</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.121316814159292</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.1132672566371681</v>
-      </c>
-      <c r="O8" t="n">
-        <v>17</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" t="n">
-        <v>0</v>
-      </c>
-      <c r="S8" t="n">
-        <v>1</v>
-      </c>
-      <c r="T8" t="n">
-        <v>0.8405345132743363</v>
-      </c>
-      <c r="U8" t="n">
-        <v>0</v>
-      </c>
-      <c r="V8" t="n">
-        <v>0</v>
-      </c>
-      <c r="W8" t="n">
-        <v>0</v>
-      </c>
-      <c r="X8" t="n">
-        <v>0.1593522123893805</v>
-      </c>
+          <t>unidentified</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">

</xml_diff>